<commit_message>
more level tidy ups
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder Dungeon World.xlsx
+++ b/darkworld/model/data/floor builder Dungeon World.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD62967-2E21-47C3-9024-923653C53283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84F773A-879E-46B8-8186-F1423B223536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="2640" windowWidth="25065" windowHeight="15840" tabRatio="904" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="2640" windowWidth="25065" windowHeight="15840" tabRatio="904" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -3040,7 +3040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2223F4-5750-492B-B43A-B4F0409B9355}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -3597,13 +3597,13 @@
         <v>4</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>4</v>
@@ -3612,10 +3612,10 @@
         <v>4</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>4</v>
@@ -3645,11 +3645,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">      fff     fffff </v>
+        <v xml:space="preserve">           ** fffff </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'      fff     fffff ',</v>
+        <v>'           ** fffff ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -3822,13 +3822,13 @@
         <v>4</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>4</v>
@@ -3837,10 +3837,10 @@
         <v>4</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>4</v>
@@ -3870,11 +3870,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">      fff           </v>
+        <v xml:space="preserve">           **       </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'      fff           ',</v>
+        <v>'           **       ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -6506,8 +6506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F10457-F664-48AB-9F9C-2CC7C0CBB34E}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6784,10 +6784,10 @@
         <v>4</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="P4" s="12" t="s">
         <v>4</v>
@@ -6811,11 +6811,11 @@
       <c r="Y4" s="7"/>
       <c r="AA4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">             __     </v>
       </c>
       <c r="AB4" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'             __     ',</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -7060,10 +7060,10 @@
         <v>4</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>4</v>
@@ -7072,10 +7072,10 @@
         <v>4</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="L8" s="12" t="s">
         <v>61</v>
@@ -7111,11 +7111,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     __  ______     </v>
+        <v xml:space="preserve">           ____     </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'     __  ______     ',</v>
+        <v>'           ____     ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -7228,10 +7228,10 @@
         <v>61</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>4</v>
@@ -7261,11 +7261,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">     ______         </v>
+        <v xml:space="preserve">     ________       </v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'     ______         ',</v>
+        <v>'     ________       ',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -26781,7 +26781,7 @@
         <v>55</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>55</v>
@@ -26817,11 +26817,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">        ;; ;;;    ;;</v>
+        <v xml:space="preserve">        ;;;;;;    ;;</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'        ;; ;;;    ;;',</v>
+        <v>'        ;;;;;;    ;;',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -26859,10 +26859,10 @@
         <v>55</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>55</v>
@@ -26892,11 +26892,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">         ;;;*;     ;</v>
+        <v xml:space="preserve">         ;;  ;     ;</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'         ;;;*;     ;',</v>
+        <v>'         ;;  ;     ;',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -27084,10 +27084,10 @@
         <v>55</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>55</v>
@@ -27117,11 +27117,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">       q ;;;;;      </v>
+        <v xml:space="preserve">       q ;;  ;      </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'       q ;;;;;      ',</v>
+        <v>'       q ;;  ;      ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -27156,16 +27156,16 @@
         <v>55</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="O12" s="12" t="s">
         <v>4</v>
@@ -27192,11 +27192,11 @@
       <c r="Y12" s="7"/>
       <c r="AA12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">        ;;          </v>
+        <v xml:space="preserve">        ;;;;;;      </v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="1"/>
-        <v>'        ;;          ',</v>
+        <v>'        ;;;;;;      ',</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>